<commit_message>
Third commit for today
</commit_message>
<xml_diff>
--- a/src/test/resources/config-and-locators.xlsx
+++ b/src/test/resources/config-and-locators.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anupreet.singh\Downloads\cucumber-pom-demo\cucumber-pom-demo\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D476FC11-CBD2-45E4-B1EA-7C7A9FD1A861}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53C1FB00-BB29-4A58-962F-C77B8C18455D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="47">
   <si>
     <t>Key</t>
   </si>
@@ -107,13 +107,73 @@
   </si>
   <si>
     <t>//span[text()='Products']</t>
+  </si>
+  <si>
+    <t>login_partnerCode</t>
+  </si>
+  <si>
+    <t>testmanager</t>
+  </si>
+  <si>
+    <t>login_username</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>login_password</t>
+  </si>
+  <si>
+    <t>Test@123456</t>
+  </si>
+  <si>
+    <t>https://ipacslegacyai-dev-qa.azurewebsites.net/</t>
+  </si>
+  <si>
+    <t>dashboard_expectedTitle</t>
+  </si>
+  <si>
+    <t>Provana IPACS – IPACS</t>
+  </si>
+  <si>
+    <t>login_partnerCodeField</t>
+  </si>
+  <si>
+    <t>partnerCode</t>
+  </si>
+  <si>
+    <t>login_usernameField</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>login_passwordField</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>login_loginButton</t>
+  </si>
+  <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>dashboard_homeNav</t>
+  </si>
+  <si>
+    <t>login_url</t>
+  </si>
+  <si>
+    <t>home_link</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -133,6 +193,29 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial Unicode MS"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -158,10 +241,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -175,8 +259,18 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -455,19 +549,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="30.54296875" defaultRowHeight="20" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="30.54296875" defaultRowHeight="36.5" customHeight="1"/>
   <cols>
     <col min="1" max="16384" width="30.54296875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="20" customHeight="1">
+    <row r="1" spans="1:3" ht="36.5" customHeight="1">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -476,7 +570,7 @@
       </c>
       <c r="C1" s="1"/>
     </row>
-    <row r="2" spans="1:3" ht="20" customHeight="1">
+    <row r="2" spans="1:3" ht="36.5" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -485,7 +579,7 @@
       </c>
       <c r="C2" s="1"/>
     </row>
-    <row r="3" spans="1:3" ht="20" customHeight="1">
+    <row r="3" spans="1:3" ht="36.5" customHeight="1">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -494,7 +588,7 @@
       </c>
       <c r="C3" s="1"/>
     </row>
-    <row r="4" spans="1:3" ht="20" customHeight="1">
+    <row r="4" spans="1:3" ht="36.5" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -503,7 +597,7 @@
       </c>
       <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="1:3" ht="20" customHeight="1">
+    <row r="5" spans="1:3" ht="36.5" customHeight="1">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -512,7 +606,7 @@
       </c>
       <c r="C5" s="1"/>
     </row>
-    <row r="6" spans="1:3" ht="20" customHeight="1">
+    <row r="6" spans="1:3" ht="36.5" customHeight="1">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
@@ -521,97 +615,190 @@
       </c>
       <c r="C6" s="1"/>
     </row>
+    <row r="7" spans="1:3" ht="36.5" customHeight="1">
+      <c r="A7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="36.5" customHeight="1">
+      <c r="A8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="36.5" customHeight="1">
+      <c r="A9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="36.5" customHeight="1">
+      <c r="A10" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="36.5" customHeight="1">
+      <c r="A11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B10" r:id="rId1" xr:uid="{B0D3C81B-EF00-4D2D-A5F4-45BA2C22795E}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77562141-90E9-4CC4-A2A9-927B24F0A282}">
-  <dimension ref="A7:D12"/>
+  <dimension ref="A7:C17"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A7" sqref="A7"/>
-      <selection pane="bottomLeft" activeCell="A7" sqref="A7:C7"/>
+      <selection pane="bottomLeft" activeCell="B17" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.6328125" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="16384" width="16.6328125" style="3"/>
+    <col min="1" max="1" width="16.6328125" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="16.6328125" style="1"/>
   </cols>
   <sheetData>
-    <row r="7" spans="1:4">
-      <c r="A7" s="4" t="s">
+    <row r="7" spans="1:3">
+      <c r="A7" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="1"/>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="1" t="s">
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="1"/>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="1" t="s">
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="1"/>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="1" t="s">
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D10" s="1"/>
-    </row>
-    <row r="11" spans="1:4" ht="29">
-      <c r="A11" s="1" t="s">
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="D11" s="1"/>
-    </row>
-    <row r="12" spans="1:4" ht="29">
-      <c r="A12" s="1" t="s">
+    </row>
+    <row r="12" spans="1:3" ht="26">
+      <c r="A12" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="D12" s="1"/>
+    </row>
+    <row r="13" spans="1:3" ht="29">
+      <c r="A13" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="29">
+      <c r="A14" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="29">
+      <c r="A15" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="29">
+      <c r="A17" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>46</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>